<commit_message>
wohngeld test for hhsize 6 added in order to increase test coverage
</commit_message>
<xml_diff>
--- a/gettsim/tests/test_data/test_dfs_wg.xlsx
+++ b/gettsim/tests/test_data/test_dfs_wg.xlsx
@@ -34,7 +34,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -45,7 +44,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">für das arbeitende Kind</t>
         </r>
@@ -60,7 +58,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -71,7 +68,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">für Behinderung
 </t>
@@ -87,7 +83,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -98,7 +93,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">für Alleinerziehende mit 1 Kind unter 11 Jahren
 </t>
@@ -114,7 +108,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -125,7 +118,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -142,7 +134,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -153,7 +144,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -170,7 +160,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -181,7 +170,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -198,7 +186,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -209,7 +196,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -226,7 +212,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -237,7 +222,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -254,7 +238,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">RS:
 </t>
@@ -265,7 +248,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">WoGG Anlage 1 (zu §19 (1))
 - zuletzt geändert durch BGBl Nr.38 vom 08.10.2015, S.1617
@@ -420,13 +402,12 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -445,21 +426,96 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,17 +524,74 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF9BBB59"/>
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -496,7 +609,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,13 +633,64 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,7 +698,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,11 +714,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,33 +726,58 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -600,7 +789,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -616,7 +805,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF9BBB59"/>
@@ -643,10 +832,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR17"/>
+  <dimension ref="A1:AR20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO15" activeCellId="0" sqref="AO15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -803,8 +992,7 @@
       <c r="C2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -817,8 +1005,7 @@
         <f aca="false">F2</f>
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -827,8 +1014,7 @@
       <c r="J2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="0" t="n">
@@ -944,8 +1130,7 @@
       <c r="C3" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -958,8 +1143,7 @@
         <f aca="false">F3</f>
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="0" t="n">
@@ -968,8 +1152,7 @@
       <c r="J3" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L3" s="0" t="n">
@@ -1085,8 +1268,7 @@
       <c r="C4" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -1099,8 +1281,7 @@
         <f aca="false">F4</f>
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="H4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="0" t="n">
@@ -1109,8 +1290,7 @@
       <c r="J4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="0" t="n">
@@ -1226,8 +1406,7 @@
       <c r="C5" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="n">
@@ -1240,8 +1419,7 @@
         <f aca="false">F5</f>
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="7" t="n">
@@ -1250,8 +1428,7 @@
       <c r="J5" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="K5" s="7" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="7" t="n">
@@ -1368,8 +1545,7 @@
       <c r="C6" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -1382,8 +1558,7 @@
         <f aca="false">F6</f>
         <v>2</v>
       </c>
-      <c r="H6" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="10" t="n">
@@ -1392,8 +1567,7 @@
       <c r="J6" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="K6" s="10" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L6" s="10" t="n">
@@ -1509,8 +1683,7 @@
       <c r="C7" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="n">
@@ -1523,8 +1696,7 @@
         <f aca="false">F7</f>
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="7" t="n">
@@ -1533,8 +1705,7 @@
       <c r="J7" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="K7" s="7" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="K7" s="11" t="b">
         <v>1</v>
       </c>
       <c r="L7" s="7" t="n">
@@ -1651,8 +1822,7 @@
       <c r="C8" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -1665,8 +1835,7 @@
         <f aca="false">F8</f>
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="H8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="9" t="n">
@@ -1675,8 +1844,7 @@
       <c r="J8" s="9" t="n">
         <v>80</v>
       </c>
-      <c r="K8" s="0" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="K8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="L8" s="9" t="n">
@@ -1792,8 +1960,7 @@
       <c r="C9" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="n">
@@ -1806,8 +1973,7 @@
         <f aca="false">F9</f>
         <v>5</v>
       </c>
-      <c r="H9" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I9" s="7" t="n">
@@ -1816,8 +1982,7 @@
       <c r="J9" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="K9" s="7" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K9" s="11" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="7" t="n">
@@ -1933,8 +2098,7 @@
       <c r="C10" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -1947,8 +2111,7 @@
         <f aca="false">F10</f>
         <v>5</v>
       </c>
-      <c r="H10" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="9" t="n">
@@ -1957,8 +2120,7 @@
       <c r="J10" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="K10" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L10" s="9" t="n">
@@ -2073,8 +2235,7 @@
       <c r="C11" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
@@ -2087,8 +2248,7 @@
         <f aca="false">F11</f>
         <v>5</v>
       </c>
-      <c r="H11" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="H11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I11" s="9" t="n">
@@ -2097,8 +2257,7 @@
       <c r="J11" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L11" s="9" t="n">
@@ -2213,8 +2372,7 @@
       <c r="C12" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
@@ -2227,8 +2385,7 @@
         <f aca="false">F12</f>
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="H12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="9" t="n">
@@ -2237,8 +2394,7 @@
       <c r="J12" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L12" s="9" t="n">
@@ -2353,8 +2509,7 @@
       <c r="C13" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
@@ -2367,8 +2522,7 @@
         <f aca="false">F13</f>
         <v>5</v>
       </c>
-      <c r="H13" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="H13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="9" t="n">
@@ -2377,8 +2531,7 @@
       <c r="J13" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="K13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L13" s="9" t="n">
@@ -2493,8 +2646,7 @@
       <c r="C14" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="n">
@@ -2506,8 +2658,7 @@
       <c r="G14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="0" t="n">
@@ -2516,7 +2667,7 @@
       <c r="J14" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L14" s="0" t="n">
@@ -2621,14 +2772,808 @@
         <v>482</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AE15" s="1"/>
+    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <f aca="false">12*O15-1000</f>
+        <v>35000</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <f aca="false">0.2*V15</f>
+        <v>7000</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <f aca="false">0.1*O15</f>
+        <v>300</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <f aca="false">0.085*O15</f>
+        <v>255</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE15" s="3" t="n">
+        <f aca="false">(AR15-((AL15+(AM15*AR15)+(AN15*AQ15))*AQ15))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG15" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH15" s="4" t="n">
+        <f aca="false">(U15+V15+W15+X15)/12+R15+S15+(P15*Q15)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AI15" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="5" t="n">
+        <f aca="false">MAX((1-AG15)*(AI15-AJ15),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL15" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM15" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN15" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO15" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ15" s="5" t="n">
+        <f aca="false">AK15</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR15" s="0" t="n">
+        <f aca="false">MIN(MAX(I15,AP15),AO15)</f>
+        <v>935</v>
+      </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AE16" s="1"/>
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE16" s="3" t="n">
+        <f aca="false">(AR16-((AL16+(AM16*AR16)+(AN16*AQ16))*AQ16))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG16" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="5" t="n">
+        <f aca="false">MAX((1-AG16)*(AI16-AJ16),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL16" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM16" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN16" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO16" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ16" s="5" t="n">
+        <f aca="false">AK16</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR16" s="0" t="n">
+        <f aca="false">MIN(MAX(I16,AP16),AO16)</f>
+        <v>935</v>
+      </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AE17" s="1"/>
+    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE17" s="3" t="n">
+        <f aca="false">(AR17-((AL17+(AM17*AR17)+(AN17*AQ17))*AQ17))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG17" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="5" t="n">
+        <f aca="false">MAX((1-AG17)*(AI17-AJ17),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL17" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM17" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN17" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO17" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ17" s="5" t="n">
+        <f aca="false">AK17</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR17" s="0" t="n">
+        <f aca="false">MIN(MAX(I17,AP17),AO17)</f>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE18" s="3" t="n">
+        <f aca="false">(AR18-((AL18+(AM18*AR18)+(AN18*AQ18))*AQ18))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG18" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="5" t="n">
+        <f aca="false">MAX((1-AG18)*(AI18-AJ18),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM18" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN18" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO18" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ18" s="5" t="n">
+        <f aca="false">AK18</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR18" s="0" t="n">
+        <f aca="false">MIN(MAX(I18,AP18),AO18)</f>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE19" s="3" t="n">
+        <f aca="false">(AR19-((AL19+(AM19*AR19)+(AN19*AQ19))*AQ19))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="5" t="n">
+        <f aca="false">MAX((1-AG19)*(AI19-AJ19),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM19" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN19" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO19" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ19" s="5" t="n">
+        <f aca="false">AK19</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR19" s="0" t="n">
+        <f aca="false">MIN(MAX(I19,AP19),AO19)</f>
+        <v>935</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="K20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="AE20" s="3" t="n">
+        <f aca="false">(AR20-((AL20+(AM20*AR20)+(AN20*AQ20))*AQ20))*1.15</f>
+        <v>41.6624683333334</v>
+      </c>
+      <c r="AG20" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="4" t="n">
+        <f aca="false">SUM($AH$15:$AH$20)</f>
+        <v>3716.66666666667</v>
+      </c>
+      <c r="AJ20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="5" t="n">
+        <f aca="false">MAX((1-AG20)*(AI20-AJ20),0)</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AL20" s="0" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="AM20" s="12" t="n">
+        <v>0.00028</v>
+      </c>
+      <c r="AN20" s="6" t="n">
+        <v>3.6E-005</v>
+      </c>
+      <c r="AO20" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="AQ20" s="5" t="n">
+        <f aca="false">AK20</f>
+        <v>2601.66666666667</v>
+      </c>
+      <c r="AR20" s="0" t="n">
+        <f aca="false">MIN(MAX(I20,AP20),AO20)</f>
+        <v>935</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>